<commit_message>
samples audio quality update
</commit_message>
<xml_diff>
--- a/Ocena utworów.xlsx
+++ b/Ocena utworów.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29512"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD1CD781-5251-4538-9C26-5161AB01C2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8F23820-A692-497C-8C4F-19995394C5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -221,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -237,6 +237,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,8 +575,8 @@
   <dimension ref="A1:N73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L55" sqref="L55"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1922,13 +1923,13 @@
         <v>13</v>
       </c>
       <c r="B39">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C39">
         <v>4</v>
       </c>
       <c r="D39">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E39">
         <v>4</v>
@@ -1953,7 +1954,7 @@
       </c>
       <c r="L39" s="6">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -1967,13 +1968,13 @@
         <v>3</v>
       </c>
       <c r="D40">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G40">
         <v>3</v>
@@ -1982,17 +1983,17 @@
         <v>2</v>
       </c>
       <c r="I40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K40">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L40" s="6">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -2003,7 +2004,7 @@
         <v>4</v>
       </c>
       <c r="C41">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D41">
         <v>4</v>
@@ -2012,7 +2013,7 @@
         <v>4</v>
       </c>
       <c r="F41">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G41">
         <v>3</v>
@@ -2031,7 +2032,7 @@
       </c>
       <c r="L41" s="6">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -2039,7 +2040,7 @@
         <v>17</v>
       </c>
       <c r="B42">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C42">
         <v>4</v>
@@ -2057,10 +2058,10 @@
         <v>3</v>
       </c>
       <c r="H42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I42">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J42">
         <v>4</v>
@@ -2070,7 +2071,7 @@
       </c>
       <c r="L42" s="6">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -2081,10 +2082,10 @@
         <v>4</v>
       </c>
       <c r="C43">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D43">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E43">
         <v>4</v>
@@ -2105,11 +2106,11 @@
         <v>4</v>
       </c>
       <c r="K43">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L43" s="6">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -3177,7 +3178,7 @@
   <dimension ref="A1:N73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
@@ -4525,16 +4526,16 @@
         <v>13</v>
       </c>
       <c r="B39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C39">
         <v>5</v>
       </c>
       <c r="D39">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39">
         <v>4</v>
@@ -4543,10 +4544,10 @@
         <v>4</v>
       </c>
       <c r="H39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J39">
         <v>4</v>
@@ -4556,7 +4557,7 @@
       </c>
       <c r="L39" s="6">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -4570,16 +4571,16 @@
         <v>4</v>
       </c>
       <c r="D40">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F40">
         <v>4</v>
       </c>
       <c r="G40">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H40">
         <v>4</v>
@@ -4588,14 +4589,14 @@
         <v>3</v>
       </c>
       <c r="J40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K40">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L40" s="6">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -4603,38 +4604,38 @@
         <v>16</v>
       </c>
       <c r="B41">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C41">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D41">
         <v>4</v>
       </c>
       <c r="E41">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F41">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G41">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H41">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J41">
         <v>3</v>
       </c>
       <c r="K41">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L41" s="6">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -4642,38 +4643,38 @@
         <v>17</v>
       </c>
       <c r="B42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C42">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D42">
         <v>4</v>
       </c>
       <c r="E42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F42">
         <v>4</v>
       </c>
       <c r="G42">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I42">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J42">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K42">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L42" s="6">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -4687,32 +4688,32 @@
         <v>4</v>
       </c>
       <c r="D43">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E43">
         <v>4</v>
       </c>
       <c r="F43">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G43">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H43">
         <v>4</v>
       </c>
       <c r="I43">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J43">
         <v>4</v>
       </c>
       <c r="K43">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L43" s="6">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -6923,29 +6924,29 @@
         <v>3</v>
       </c>
       <c r="E33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I33">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L33" s="6">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -7125,38 +7126,38 @@
         <v>13</v>
       </c>
       <c r="B39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G39">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J39">
         <v>3</v>
       </c>
       <c r="K39">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L39" s="6">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -7164,16 +7165,16 @@
         <v>15</v>
       </c>
       <c r="B40">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C40">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E40">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F40">
         <v>4</v>
@@ -7182,20 +7183,20 @@
         <v>3</v>
       </c>
       <c r="H40">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I40">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J40">
         <v>4</v>
       </c>
       <c r="K40">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L40" s="6">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -7203,7 +7204,7 @@
         <v>16</v>
       </c>
       <c r="B41">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C41">
         <v>5</v>
@@ -7215,16 +7216,16 @@
         <v>4</v>
       </c>
       <c r="F41">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G41">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H41">
         <v>4</v>
       </c>
       <c r="I41">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J41">
         <v>4</v>
@@ -7234,7 +7235,7 @@
       </c>
       <c r="L41" s="6">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -7242,22 +7243,22 @@
         <v>17</v>
       </c>
       <c r="B42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C42">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D42">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E42">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F42">
         <v>4</v>
       </c>
       <c r="G42">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H42">
         <v>4</v>
@@ -7266,14 +7267,14 @@
         <v>4</v>
       </c>
       <c r="J42">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K42">
         <v>7</v>
       </c>
       <c r="L42" s="6">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -7281,7 +7282,7 @@
         <v>18</v>
       </c>
       <c r="B43">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C43">
         <v>4</v>
@@ -7290,29 +7291,29 @@
         <v>4</v>
       </c>
       <c r="E43">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F43">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G43">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H43">
         <v>4</v>
       </c>
       <c r="I43">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J43">
         <v>4</v>
       </c>
       <c r="K43">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L43" s="6">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -8664,7 +8665,7 @@
       </c>
       <c r="B33" s="6">
         <f>SUM(MB!L33,SK!L33,JW!L33)</f>
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -8715,7 +8716,7 @@
       </c>
       <c r="B39" s="6">
         <f>SUM(MB!L39,SK!L39,JW!L39)</f>
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -8724,7 +8725,7 @@
       </c>
       <c r="B40" s="6">
         <f>SUM(MB!L40,SK!L40,JW!L40)</f>
-        <v>129</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -8733,7 +8734,7 @@
       </c>
       <c r="B41" s="6">
         <f>SUM(MB!L41,SK!L41,JW!L41)</f>
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -8742,7 +8743,7 @@
       </c>
       <c r="B42" s="6">
         <f>SUM(MB!L42,SK!L42,JW!L42)</f>
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -8751,7 +8752,7 @@
       </c>
       <c r="B43" s="6">
         <f>SUM(MB!L43,SK!L43,JW!L43)</f>
-        <v>119</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -9018,8 +9019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4498410-1457-468C-A43D-8EDEE490875E}">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9062,12 +9063,12 @@
         <v>34</v>
       </c>
       <c r="C3">
-        <f>ROUND(9 * 25/12, 0)</f>
-        <v>19</v>
+        <f>ROUND(9 * 25/14, 0)</f>
+        <v>16</v>
       </c>
       <c r="D3" s="6">
         <f>SUM(B3,C3)</f>
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>33</v>
@@ -9082,12 +9083,12 @@
         <v>43</v>
       </c>
       <c r="C4">
-        <f>ROUND(9 * 25/12, 0)</f>
-        <v>19</v>
+        <f>ROUND(9 * 25/14, 0)</f>
+        <v>16</v>
       </c>
       <c r="D4" s="6">
         <f t="shared" ref="D4:D66" si="0">SUM(B4,C4)</f>
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -9099,12 +9100,12 @@
         <v>45</v>
       </c>
       <c r="C5">
-        <f>ROUND(11 * 25/12, 0)</f>
-        <v>23</v>
+        <f>ROUND(11 * 25/14, 0)</f>
+        <v>20</v>
       </c>
       <c r="D5" s="12">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -9116,12 +9117,12 @@
         <v>41</v>
       </c>
       <c r="C6">
-        <f>ROUND(11 * 25/12, 0)</f>
-        <v>23</v>
+        <f>ROUND(11 * 25/14, 0)</f>
+        <v>20</v>
       </c>
       <c r="D6" s="6">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -9133,12 +9134,12 @@
         <v>41</v>
       </c>
       <c r="C7">
-        <f>ROUND(11 * 25/12, 0)</f>
-        <v>23</v>
+        <f>ROUND(11 * 25/14, 0)</f>
+        <v>20</v>
       </c>
       <c r="D7" s="6">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -9158,12 +9159,12 @@
         <v>39</v>
       </c>
       <c r="C9">
-        <f>ROUND(9 * 25/12, 0)</f>
-        <v>19</v>
+        <f>ROUND(9 * 25/14, 0)</f>
+        <v>16</v>
       </c>
       <c r="D9" s="6">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -9175,12 +9176,12 @@
         <v>35</v>
       </c>
       <c r="C10">
-        <f>ROUND(8 * 25/12, 0)</f>
-        <v>17</v>
+        <f>ROUND(8 * 25/14, 0)</f>
+        <v>14</v>
       </c>
       <c r="D10" s="6">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -9192,12 +9193,12 @@
         <v>33</v>
       </c>
       <c r="C11">
-        <f>ROUND(8 * 25/12, 0)</f>
-        <v>17</v>
+        <f>ROUND(8 * 25/14, 0)</f>
+        <v>14</v>
       </c>
       <c r="D11" s="6">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -9209,12 +9210,12 @@
         <v>37</v>
       </c>
       <c r="C12">
-        <f>ROUND(9 * 25/12, 0)</f>
-        <v>19</v>
+        <f>ROUND(9 * 25/14, 0)</f>
+        <v>16</v>
       </c>
       <c r="D12" s="6">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -9226,12 +9227,12 @@
         <v>45</v>
       </c>
       <c r="C13">
-        <f>ROUND(9 * 25/12, 0)</f>
-        <v>19</v>
+        <f>ROUND(9 * 25/14, 0)</f>
+        <v>16</v>
       </c>
       <c r="D13" s="12">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -9251,12 +9252,12 @@
         <v>36</v>
       </c>
       <c r="C15">
-        <f>ROUND(10 * 25/12, 0)</f>
-        <v>21</v>
+        <f>ROUND(10 * 25/14, 0)</f>
+        <v>18</v>
       </c>
       <c r="D15" s="6">
         <f t="shared" si="0"/>
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -9268,12 +9269,12 @@
         <v>45</v>
       </c>
       <c r="C16">
-        <f>ROUND(9 * 25/12, 0)</f>
-        <v>19</v>
+        <f>ROUND(9 * 25/14, 0)</f>
+        <v>16</v>
       </c>
       <c r="D16" s="12">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -9285,12 +9286,12 @@
         <v>28</v>
       </c>
       <c r="C17">
-        <f>ROUND(11 * 25/12, 0)</f>
-        <v>23</v>
+        <f>ROUND(11 * 25/14, 0)</f>
+        <v>20</v>
       </c>
       <c r="D17" s="6">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -9302,12 +9303,12 @@
         <v>32</v>
       </c>
       <c r="C18">
-        <f>ROUND(9 * 25/12, 0)</f>
-        <v>19</v>
+        <f>ROUND(9 * 25/14, 0)</f>
+        <v>16</v>
       </c>
       <c r="D18" s="6">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -9319,12 +9320,12 @@
         <v>35</v>
       </c>
       <c r="C19">
-        <f>ROUND(8 * 25/12, 0)</f>
-        <v>17</v>
+        <f>ROUND(8 * 25/14, 0)</f>
+        <v>14</v>
       </c>
       <c r="D19" s="6">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -9344,12 +9345,12 @@
         <v>26</v>
       </c>
       <c r="C21">
-        <f>ROUND(12 * 25/12, 0)</f>
-        <v>25</v>
+        <f>ROUND(12 * 25/14, 0)</f>
+        <v>21</v>
       </c>
       <c r="D21" s="6">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -9361,12 +9362,12 @@
         <v>26</v>
       </c>
       <c r="C22">
-        <f>ROUND(10 * 25/12, 0)</f>
-        <v>21</v>
+        <f>ROUND(10 * 25/14, 0)</f>
+        <v>18</v>
       </c>
       <c r="D22" s="6">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -9378,12 +9379,12 @@
         <v>35</v>
       </c>
       <c r="C23">
-        <f>ROUND(11 * 25/12, 0)</f>
-        <v>23</v>
+        <f>ROUND(11 * 25/14, 0)</f>
+        <v>20</v>
       </c>
       <c r="D23" s="6">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -9395,12 +9396,12 @@
         <v>38</v>
       </c>
       <c r="C24">
-        <f>ROUND(11 * 25/12, 0)</f>
-        <v>23</v>
+        <f>ROUND(11 * 25/14, 0)</f>
+        <v>20</v>
       </c>
       <c r="D24" s="6">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -9412,12 +9413,12 @@
         <v>41</v>
       </c>
       <c r="C25">
-        <f>ROUND(11 * 25/12, 0)</f>
-        <v>23</v>
+        <f>ROUND(11 * 25/14, 0)</f>
+        <v>20</v>
       </c>
       <c r="D25" s="12">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -9437,12 +9438,12 @@
         <v>34</v>
       </c>
       <c r="C27">
-        <f>ROUND(10 * 25/12, 0)</f>
-        <v>21</v>
+        <f>ROUND(10 * 25/14, 0)</f>
+        <v>18</v>
       </c>
       <c r="D27" s="6">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -9454,12 +9455,12 @@
         <v>39</v>
       </c>
       <c r="C28">
-        <f>ROUND(9 * 25/12, 0)</f>
-        <v>19</v>
+        <f>ROUND(9 * 25/14, 0)</f>
+        <v>16</v>
       </c>
       <c r="D28" s="6">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -9471,12 +9472,12 @@
         <v>29</v>
       </c>
       <c r="C29">
-        <f>ROUND(11 * 25/12, 0)</f>
-        <v>23</v>
+        <f>ROUND(11 * 25/14, 0)</f>
+        <v>20</v>
       </c>
       <c r="D29" s="6">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -9488,12 +9489,12 @@
         <v>34</v>
       </c>
       <c r="C30">
-        <f>ROUND(9 * 25/12, 0)</f>
-        <v>19</v>
+        <f>ROUND(9 * 25/14, 0)</f>
+        <v>16</v>
       </c>
       <c r="D30" s="6">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -9505,12 +9506,12 @@
         <v>45</v>
       </c>
       <c r="C31">
-        <f>ROUND(11 * 25/12, 0)</f>
-        <v>23</v>
+        <f>ROUND(11 * 25/14, 0)</f>
+        <v>20</v>
       </c>
       <c r="D31" s="12">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -9527,15 +9528,15 @@
       </c>
       <c r="B33">
         <f>ROUND((SUMA!B33 - 10) * 75/155,0)</f>
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C33">
-        <f>ROUND(11 * 25/12, 0)</f>
-        <v>23</v>
+        <f>ROUND(11 * 25/14, 0)</f>
+        <v>20</v>
       </c>
       <c r="D33" s="6">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -9547,12 +9548,12 @@
         <v>26</v>
       </c>
       <c r="C34">
-        <f>ROUND(9 * 25/12, 0)</f>
-        <v>19</v>
+        <f>ROUND(9 * 25/14, 0)</f>
+        <v>16</v>
       </c>
       <c r="D34" s="6">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -9564,12 +9565,12 @@
         <v>54</v>
       </c>
       <c r="C35">
-        <f>ROUND(11 * 25/12, 0)</f>
-        <v>23</v>
+        <f>ROUND(11 * 25/14, 0)</f>
+        <v>20</v>
       </c>
       <c r="D35" s="12">
         <f t="shared" si="0"/>
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -9581,12 +9582,12 @@
         <v>31</v>
       </c>
       <c r="C36">
-        <f>ROUND(11 * 25/12, 0)</f>
-        <v>23</v>
+        <f>ROUND(11 * 25/14, 0)</f>
+        <v>20</v>
       </c>
       <c r="D36" s="6">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -9598,12 +9599,12 @@
         <v>41</v>
       </c>
       <c r="C37">
-        <f>ROUND(8 * 25/12, 0)</f>
-        <v>17</v>
+        <f>ROUND(8 * 25/14, 0)</f>
+        <v>14</v>
       </c>
       <c r="D37" s="6">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -9620,15 +9621,15 @@
       </c>
       <c r="B39">
         <f>ROUND((SUMA!B39 - 10) * 75/155,0)</f>
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C39">
-        <f>ROUND(12 * 25/12, 0)</f>
-        <v>25</v>
-      </c>
-      <c r="D39" s="12">
-        <f t="shared" si="0"/>
-        <v>83</v>
+        <f>ROUND(13 * 25/14, 0)</f>
+        <v>23</v>
+      </c>
+      <c r="D39" s="13">
+        <f t="shared" si="0"/>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -9637,15 +9638,15 @@
       </c>
       <c r="B40">
         <f>ROUND((SUMA!B40 - 10) * 75/155,0)</f>
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C40">
-        <f>ROUND(11 * 25/12, 0)</f>
-        <v>23</v>
+        <f>ROUND(12 * 25/14, 0)</f>
+        <v>21</v>
       </c>
       <c r="D40" s="6">
         <f t="shared" si="0"/>
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -9654,15 +9655,15 @@
       </c>
       <c r="B41">
         <f>ROUND((SUMA!B41 - 10) * 75/155,0)</f>
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C41">
-        <f>ROUND(12 * 25/12, 0)</f>
+        <f>ROUND(14 * 25/14, 0)</f>
         <v>25</v>
       </c>
-      <c r="D41" s="6">
-        <f t="shared" si="0"/>
-        <v>79</v>
+      <c r="D41" s="12">
+        <f t="shared" si="0"/>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -9671,15 +9672,15 @@
       </c>
       <c r="B42">
         <f>ROUND((SUMA!B42 - 10) * 75/155,0)</f>
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C42">
-        <f>ROUND(10 * 25/12, 0)</f>
-        <v>21</v>
+        <f>ROUND(14 * 25/14, 0)</f>
+        <v>25</v>
       </c>
       <c r="D42" s="6">
         <f t="shared" si="0"/>
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -9688,15 +9689,15 @@
       </c>
       <c r="B43">
         <f>ROUND((SUMA!B43 - 10) * 75/155,0)</f>
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C43">
-        <f>ROUND(12 * 25/12, 0)</f>
-        <v>25</v>
+        <f>ROUND(12 * 25/14, 0)</f>
+        <v>21</v>
       </c>
       <c r="D43" s="6">
         <f t="shared" si="0"/>
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -9716,12 +9717,12 @@
         <v>54</v>
       </c>
       <c r="C45">
-        <f>ROUND(10 * 25/12, 0)</f>
-        <v>21</v>
+        <f>ROUND(11 * 25/14, 0)</f>
+        <v>20</v>
       </c>
       <c r="D45" s="6">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -9733,12 +9734,12 @@
         <v>52</v>
       </c>
       <c r="C46">
-        <f>ROUND(11 * 25/12, 0)</f>
-        <v>23</v>
+        <f>ROUND(12 * 25/14, 0)</f>
+        <v>21</v>
       </c>
       <c r="D46" s="6">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -9750,12 +9751,12 @@
         <v>57</v>
       </c>
       <c r="C47">
-        <f>ROUND(10 * 25/12, 0)</f>
-        <v>21</v>
+        <f>ROUND(11 * 25/14, 0)</f>
+        <v>20</v>
       </c>
       <c r="D47" s="12">
         <f t="shared" si="0"/>
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -9767,12 +9768,12 @@
         <v>53</v>
       </c>
       <c r="C48">
-        <f>ROUND(10 * 25/12, 0)</f>
-        <v>21</v>
+        <f>ROUND(11 * 25/14, 0)</f>
+        <v>20</v>
       </c>
       <c r="D48" s="6">
         <f t="shared" si="0"/>
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -9784,12 +9785,12 @@
         <v>56</v>
       </c>
       <c r="C49">
-        <f>ROUND(10 * 25/12, 0)</f>
-        <v>21</v>
+        <f>ROUND(11 * 25/14, 0)</f>
+        <v>20</v>
       </c>
       <c r="D49" s="6">
         <f t="shared" si="0"/>
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -9809,12 +9810,12 @@
         <v>39</v>
       </c>
       <c r="C51">
-        <f>ROUND(9 * 25/12, 0)</f>
-        <v>19</v>
+        <f>ROUND(10 * 25/14, 0)</f>
+        <v>18</v>
       </c>
       <c r="D51" s="6">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -9826,7 +9827,7 @@
         <v>52</v>
       </c>
       <c r="C52">
-        <f>ROUND(10 * 25/12, 0)</f>
+        <f>ROUND(12 * 25/14, 0)</f>
         <v>21</v>
       </c>
       <c r="D52" s="6">
@@ -9843,12 +9844,12 @@
         <v>52</v>
       </c>
       <c r="C53">
-        <f>ROUND(11 * 25/12, 0)</f>
-        <v>23</v>
+        <f>ROUND(11 * 25/14, 0)</f>
+        <v>20</v>
       </c>
       <c r="D53" s="6">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -9860,12 +9861,12 @@
         <v>52</v>
       </c>
       <c r="C54">
-        <f>ROUND(11 * 25/12, 0)</f>
-        <v>23</v>
+        <f>ROUND(12 * 25/14, 0)</f>
+        <v>21</v>
       </c>
       <c r="D54" s="6">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -9877,12 +9878,12 @@
         <v>60</v>
       </c>
       <c r="C55">
-        <f>ROUND(11 * 25/12, 0)</f>
-        <v>23</v>
+        <f>ROUND(12 * 25/14, 0)</f>
+        <v>21</v>
       </c>
       <c r="D55" s="12">
         <f t="shared" si="0"/>
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -9902,12 +9903,12 @@
         <v>57</v>
       </c>
       <c r="C57">
-        <f>ROUND(10 * 25/12, 0)</f>
-        <v>21</v>
+        <f>ROUND(10 * 25/14, 0)</f>
+        <v>18</v>
       </c>
       <c r="D57" s="12">
         <f t="shared" si="0"/>
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -9919,12 +9920,12 @@
         <v>52</v>
       </c>
       <c r="C58">
-        <f>ROUND(10 * 25/12, 0)</f>
-        <v>21</v>
+        <f>ROUND(10 * 25/14, 0)</f>
+        <v>18</v>
       </c>
       <c r="D58" s="6">
         <f t="shared" si="0"/>
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -9936,12 +9937,12 @@
         <v>54</v>
       </c>
       <c r="C59">
-        <f>ROUND(9 * 25/12, 0)</f>
-        <v>19</v>
+        <f>ROUND(9 * 25/14, 0)</f>
+        <v>16</v>
       </c>
       <c r="D59" s="6">
         <f t="shared" si="0"/>
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -9953,12 +9954,12 @@
         <v>55</v>
       </c>
       <c r="C60">
-        <f>ROUND(9 * 25/12, 0)</f>
-        <v>19</v>
+        <f>ROUND(9 * 25/14, 0)</f>
+        <v>16</v>
       </c>
       <c r="D60" s="6">
         <f t="shared" si="0"/>
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -9970,12 +9971,12 @@
         <v>57</v>
       </c>
       <c r="C61">
-        <f>ROUND(8 * 25/12, 0)</f>
-        <v>17</v>
+        <f>ROUND(8 * 25/14, 0)</f>
+        <v>14</v>
       </c>
       <c r="D61" s="6">
         <f t="shared" si="0"/>
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -9995,12 +9996,12 @@
         <v>52</v>
       </c>
       <c r="C63">
-        <f>ROUND(9 * 25/12, 0)</f>
-        <v>19</v>
+        <f>ROUND(9 * 25/14, 0)</f>
+        <v>16</v>
       </c>
       <c r="D63" s="12">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -10012,12 +10013,12 @@
         <v>47</v>
       </c>
       <c r="C64">
-        <f>ROUND(6 * 25/12, 0)</f>
-        <v>13</v>
+        <f>ROUND(6 * 25/14, 0)</f>
+        <v>11</v>
       </c>
       <c r="D64" s="6">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -10029,12 +10030,12 @@
         <v>44</v>
       </c>
       <c r="C65">
-        <f>ROUND(7 * 25/12, 0)</f>
-        <v>15</v>
+        <f>ROUND(7 * 25/14, 0)</f>
+        <v>13</v>
       </c>
       <c r="D65" s="6">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -10046,12 +10047,12 @@
         <v>50</v>
       </c>
       <c r="C66">
-        <f>ROUND(7 * 25/12, 0)</f>
-        <v>15</v>
+        <f>ROUND(7 * 25/14, 0)</f>
+        <v>13</v>
       </c>
       <c r="D66" s="6">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -10063,12 +10064,12 @@
         <v>48</v>
       </c>
       <c r="C67">
-        <f>ROUND(8 * 25/12, 0)</f>
-        <v>17</v>
+        <f>ROUND(8 * 25/14, 0)</f>
+        <v>14</v>
       </c>
       <c r="D67" s="6">
         <f>SUM(B67,C67)</f>
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -10088,12 +10089,12 @@
         <v>51</v>
       </c>
       <c r="C69">
-        <f>ROUND(11 * 25/12, 0)</f>
-        <v>23</v>
+        <f>ROUND(11 * 25/14, 0)</f>
+        <v>20</v>
       </c>
       <c r="D69" s="6">
         <f t="shared" ref="D69:D73" si="1">SUM(B69,C69)</f>
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -10105,12 +10106,12 @@
         <v>53</v>
       </c>
       <c r="C70">
-        <f>ROUND(11 * 25/12, 0)</f>
-        <v>23</v>
+        <f>ROUND(11 * 25/14, 0)</f>
+        <v>20</v>
       </c>
       <c r="D70" s="6">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -10122,12 +10123,12 @@
         <v>47</v>
       </c>
       <c r="C71">
-        <f>ROUND(11 * 25/12, 0)</f>
-        <v>23</v>
+        <f>ROUND(11 * 25/14, 0)</f>
+        <v>20</v>
       </c>
       <c r="D71" s="6">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -10139,12 +10140,12 @@
         <v>50</v>
       </c>
       <c r="C72">
-        <f>ROUND(10 * 25/12, 0)</f>
-        <v>21</v>
+        <f>ROUND(10 * 25/14, 0)</f>
+        <v>18</v>
       </c>
       <c r="D72" s="6">
         <f t="shared" si="1"/>
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -10156,12 +10157,12 @@
         <v>55</v>
       </c>
       <c r="C73">
-        <f>ROUND(12 * 25/12, 0)</f>
-        <v>25</v>
+        <f>ROUND(12 * 25/14, 0)</f>
+        <v>21</v>
       </c>
       <c r="D73" s="12">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>